<commit_message>
all the problem can show
</commit_message>
<xml_diff>
--- a/data/problem.xlsx
+++ b/data/problem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\2021_summer\python_en\bank\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60D3A60-54B9-4D26-83A5-2DB3D416A4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D00929F-9AAA-4F70-8CC6-9A67A0F16926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="信息" sheetId="4" r:id="rId1"/>
@@ -855,10 +855,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>列表对象的排序方法sort()()只能按元素从小到大排列,不支持别的排序方式。</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>形参可以看做是函数内部的局部变量,函数运行结束之后形参就不可访问了</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -1667,6 +1663,10 @@
 2.不能用关键字。</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>列表对象的排序方法sort()只能按元素从小到大排列,不支持别的排序方式。</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2132,7 +2132,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="I8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3326,8 +3326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F44210-511C-4C3E-8E1C-96686BF49A00}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3366,7 +3366,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>246</v>
+        <v>318</v>
       </c>
       <c r="C2" s="3" t="b">
         <v>1</v>
@@ -3377,10 +3377,10 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
@@ -3388,7 +3388,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>1</v>
@@ -3399,7 +3399,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H3" s="3"/>
     </row>
@@ -3408,7 +3408,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>1</v>
@@ -3419,7 +3419,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H4" s="3"/>
     </row>
@@ -3428,7 +3428,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C5" s="3" t="b">
         <v>1</v>
@@ -3439,7 +3439,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -3448,7 +3448,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C6" s="3" t="b">
         <v>1</v>
@@ -3459,7 +3459,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -3468,7 +3468,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C7" s="3" t="b">
         <v>1</v>
@@ -3479,7 +3479,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -3488,7 +3488,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C8" s="3" t="b">
         <v>1</v>
@@ -3499,7 +3499,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H8" s="3"/>
     </row>
@@ -3508,7 +3508,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C9" s="3" t="b">
         <v>1</v>
@@ -3519,7 +3519,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -3528,7 +3528,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C10" s="3" t="b">
         <v>1</v>
@@ -3539,7 +3539,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H10" s="3"/>
     </row>
@@ -3548,7 +3548,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C11" s="3" t="b">
         <v>1</v>
@@ -3559,7 +3559,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -3568,7 +3568,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>1</v>
@@ -3579,7 +3579,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -3588,7 +3588,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>1</v>
@@ -3599,7 +3599,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -3608,7 +3608,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>1</v>
@@ -3619,7 +3619,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H14" s="3"/>
     </row>
@@ -3628,7 +3628,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>1</v>
@@ -3639,7 +3639,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H15" s="3"/>
     </row>
@@ -3648,7 +3648,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C16" s="3" t="b">
         <v>1</v>
@@ -3659,7 +3659,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H16" s="3"/>
     </row>
@@ -3668,7 +3668,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C17" s="3" t="b">
         <v>1</v>
@@ -3679,7 +3679,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H17" s="3"/>
     </row>
@@ -3688,7 +3688,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C18" s="3" t="b">
         <v>1</v>
@@ -3699,7 +3699,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H18" s="3"/>
     </row>
@@ -3708,7 +3708,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C19" s="3" t="b">
         <v>1</v>
@@ -3719,7 +3719,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H19" s="3"/>
     </row>
@@ -3728,7 +3728,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C20" s="3" t="b">
         <v>1</v>
@@ -3739,7 +3739,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H20" s="3"/>
     </row>
@@ -3748,7 +3748,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C21" s="3" t="b">
         <v>1</v>
@@ -3759,7 +3759,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H21" s="3"/>
     </row>
@@ -3768,7 +3768,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C22" s="3" t="b">
         <v>1</v>
@@ -3779,7 +3779,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H22" s="3"/>
     </row>
@@ -3788,7 +3788,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C23" s="3" t="b">
         <v>1</v>
@@ -3799,7 +3799,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H23" s="3"/>
     </row>
@@ -3808,7 +3808,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C24" s="3" t="b">
         <v>1</v>
@@ -3819,7 +3819,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H24" s="3"/>
     </row>
@@ -3828,7 +3828,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C25" s="3" t="b">
         <v>1</v>
@@ -3839,7 +3839,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H25" s="3"/>
     </row>
@@ -3848,7 +3848,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C26" s="3" t="b">
         <v>1</v>
@@ -3859,7 +3859,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H26" s="3"/>
     </row>
@@ -3868,7 +3868,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C27" s="3" t="b">
         <v>1</v>
@@ -3879,7 +3879,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H27" s="3"/>
     </row>
@@ -3888,7 +3888,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C28" s="3" t="b">
         <v>1</v>
@@ -3899,7 +3899,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H28" s="3"/>
     </row>
@@ -3908,7 +3908,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C29" s="3" t="b">
         <v>1</v>
@@ -3919,7 +3919,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H29" s="3"/>
     </row>
@@ -3928,7 +3928,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C30" s="3" t="b">
         <v>1</v>
@@ -3939,7 +3939,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H30" s="3"/>
     </row>
@@ -3948,7 +3948,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C31" s="3" t="b">
         <v>1</v>
@@ -3959,7 +3959,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H31" s="3"/>
     </row>
@@ -3968,7 +3968,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C32" s="3" t="b">
         <v>1</v>
@@ -3979,7 +3979,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H32" s="3"/>
     </row>
@@ -3988,7 +3988,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C33" s="3" t="b">
         <v>1</v>
@@ -3999,7 +3999,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H33" s="3"/>
     </row>
@@ -4008,7 +4008,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C34" s="3" t="b">
         <v>1</v>
@@ -4019,7 +4019,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H34" s="3"/>
     </row>
@@ -4028,7 +4028,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C35" s="3" t="b">
         <v>1</v>
@@ -4039,7 +4039,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H35" s="3"/>
     </row>
@@ -4048,7 +4048,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C36" s="3" t="b">
         <v>1</v>
@@ -4059,7 +4059,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H36" s="3"/>
     </row>
@@ -4068,7 +4068,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C37" s="3" t="b">
         <v>1</v>
@@ -4079,7 +4079,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H37" s="3"/>
     </row>
@@ -4088,7 +4088,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C38" s="3" t="b">
         <v>1</v>
@@ -4099,7 +4099,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H38" s="3"/>
     </row>
@@ -4108,7 +4108,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C39" s="3" t="b">
         <v>1</v>
@@ -4119,7 +4119,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H39" s="3"/>
     </row>
@@ -4128,7 +4128,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C40" s="3" t="b">
         <v>1</v>
@@ -4139,7 +4139,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H40" s="3"/>
     </row>
@@ -4148,7 +4148,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C41" s="3" t="b">
         <v>1</v>
@@ -4159,7 +4159,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H41" s="3"/>
     </row>
@@ -4168,7 +4168,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C42" s="3" t="b">
         <v>1</v>
@@ -4179,7 +4179,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H42" s="3"/>
     </row>
@@ -4188,7 +4188,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C43" s="3" t="b">
         <v>1</v>
@@ -4199,7 +4199,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H43" s="3"/>
     </row>
@@ -4208,7 +4208,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C44" s="3" t="b">
         <v>1</v>
@@ -4219,7 +4219,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H44" s="3"/>
     </row>
@@ -4228,7 +4228,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C45" s="3" t="b">
         <v>1</v>
@@ -4239,7 +4239,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H45" s="3"/>
     </row>
@@ -4248,7 +4248,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C46" s="3" t="b">
         <v>1</v>
@@ -4259,7 +4259,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H46" s="3"/>
     </row>
@@ -4268,7 +4268,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C47" s="3" t="b">
         <v>1</v>
@@ -4279,7 +4279,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H47" s="3"/>
     </row>
@@ -4288,7 +4288,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C48" s="3" t="b">
         <v>1</v>
@@ -4299,7 +4299,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H48" s="3"/>
     </row>
@@ -4308,7 +4308,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C49" s="3" t="b">
         <v>1</v>
@@ -4319,7 +4319,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H49" s="3"/>
     </row>
@@ -4328,7 +4328,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C50" s="3" t="b">
         <v>1</v>
@@ -4339,7 +4339,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H50" s="3"/>
     </row>
@@ -4348,7 +4348,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C51" s="3" t="b">
         <v>1</v>
@@ -4359,13 +4359,14 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H51" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4373,7 +4374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134F5492-ECD4-4955-AD80-281E493258CE}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -4410,14 +4411,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.4">
@@ -4425,14 +4426,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.4">
@@ -4440,14 +4441,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.4">
@@ -4455,14 +4456,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.4">
@@ -4470,14 +4471,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.4">
@@ -4485,14 +4486,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.4">
@@ -4500,14 +4501,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.4">
@@ -4515,14 +4516,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.4">
@@ -4530,14 +4531,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.4">
@@ -4545,14 +4546,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>